<commit_message>
Added: CSS_210/M2 CSS_210/M3 MTH_102/M1 MTH_102/M2 MTH_102/M3 MTH_102/M4
</commit_message>
<xml_diff>
--- a/MTH_102/Module01/M1 ICA.xlsx
+++ b/MTH_102/Module01/M1 ICA.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lucas/Desktop/National Louis/SU25 MTH102/Module 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ishrak\Workspace\nl-css-coursework\MTH_102\Module01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0A3643-0E3F-F34F-BD95-4C535D2FAE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC17C060-42C2-4100-9EEE-30F121B33611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Line Graph" sheetId="5" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="21">
   <si>
     <t>Hospt</t>
   </si>
@@ -88,6 +91,15 @@
   </si>
   <si>
     <t>Your pivot table and pie chart for Exercises 2 to 4 should go somewhere below this text.</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Hospt</t>
   </si>
 </sst>
 </file>
@@ -299,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -324,6 +336,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -376,6 +393,3576 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Employees in</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> each month</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2198531435649216E-2"/>
+          <c:y val="0.19251110251165529"/>
+          <c:w val="0.89668540419042342"/>
+          <c:h val="0.72425356135103547"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Line Graph'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># of Employees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Line Graph'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Line Graph'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F779-4F5C-A31F-578354A7F35C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="703390480"/>
+        <c:axId val="703407280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="703390480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="703407280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="703407280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Employees</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="703390480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Ishrak Rahman.xlsx]Data!PivotTable1</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Distribution of Participants of Treatment by Hospital</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:pattFill prst="pct75">
+              <a:fgClr>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:sysClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-E5D1-420C-9D9B-CD017D8A65C3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-E5D1-420C-9D9B-CD017D8A65C3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-E5D1-420C-9D9B-CD017D8A65C3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-E5D1-420C-9D9B-CD017D8A65C3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-E5D1-420C-9D9B-CD017D8A65C3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:sysClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$I$4:$I$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$J$4:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.16513761467889909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15596330275229359</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1743119266055051E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34862385321100919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23853211009174313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DC65-462F-B489-A262D79E1C58}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>698464</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC3EF4AB-DD2D-8734-520C-10AA844CF8DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142240</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A099B752-912C-7A76-B1B6-0067DB2B07C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ishrak" refreshedDate="45845.459625115742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="109" xr:uid="{83C72C29-8F91-4641-87D1-F7AED898B48F}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:G110" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Hospt" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5" count="5">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Treat" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Outcome" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Time" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="206"/>
+    </cacheField>
+    <cacheField name="D-Time" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="47" maxValue="512"/>
+    </cacheField>
+    <cacheField name="Age" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="20" maxValue="65"/>
+    </cacheField>
+    <cacheField name="Sex" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="109">
+  <r>
+    <x v="0"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="36.143000000000001"/>
+    <n v="211"/>
+    <n v="33"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="105.143"/>
+    <n v="176"/>
+    <n v="49"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="74.570999999999998"/>
+    <n v="191"/>
+    <n v="50"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="49.713999999999999"/>
+    <n v="206"/>
+    <n v="29"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="14.429"/>
+    <n v="63"/>
+    <n v="29"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="5"/>
+    <n v="70"/>
+    <n v="30"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="104.857"/>
+    <n v="55"/>
+    <n v="56"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="2.8570000000000002"/>
+    <n v="512"/>
+    <n v="48"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="102.429"/>
+    <n v="162"/>
+    <n v="22"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="55.713999999999999"/>
+    <n v="306"/>
+    <n v="61"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="106.429"/>
+    <n v="165"/>
+    <n v="58"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="105.143"/>
+    <n v="129"/>
+    <n v="31"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="83"/>
+    <n v="428"/>
+    <n v="44"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="27.286000000000001"/>
+    <n v="256"/>
+    <n v="55"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="105.857"/>
+    <n v="197"/>
+    <n v="57"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="5.5709999999999997"/>
+    <n v="227"/>
+    <n v="46"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="98"/>
+    <n v="168"/>
+    <n v="58"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="16.286000000000001"/>
+    <n v="194"/>
+    <n v="57"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="1.286"/>
+    <n v="173"/>
+    <n v="54"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="2.1429999999999998"/>
+    <n v="48"/>
+    <n v="23"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="100"/>
+    <n v="47"/>
+    <n v="65"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="27.143000000000001"/>
+    <n v="95"/>
+    <n v="27"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="4"/>
+    <n v="148"/>
+    <n v="50"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="74.143000000000001"/>
+    <n v="127"/>
+    <n v="41"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="104.857"/>
+    <n v="129"/>
+    <n v="65"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="0.14299999999999999"/>
+    <n v="182"/>
+    <n v="52"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="1.429"/>
+    <n v="90"/>
+    <n v="60"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="45.856999999999999"/>
+    <n v="177"/>
+    <n v="25"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="17.428999999999998"/>
+    <n v="234"/>
+    <n v="27"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="78"/>
+    <n v="322"/>
+    <n v="32"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="66.856999999999999"/>
+    <n v="141"/>
+    <n v="43"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="78.429000000000002"/>
+    <n v="165"/>
+    <n v="20"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="78.429000000000002"/>
+    <n v="239"/>
+    <n v="23"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="78.143000000000001"/>
+    <n v="147"/>
+    <n v="36"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="15.856999999999999"/>
+    <n v="348"/>
+    <n v="22"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="79"/>
+    <n v="274"/>
+    <n v="49"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="32.570999999999998"/>
+    <n v="130"/>
+    <n v="40"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="9"/>
+    <n v="98"/>
+    <n v="54"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="3.286"/>
+    <n v="77"/>
+    <n v="26"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="206"/>
+    <n v="90"/>
+    <n v="48"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="30"/>
+    <n v="280"/>
+    <n v="51"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="7.1429999999999998"/>
+    <n v="167"/>
+    <n v="35"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="31"/>
+    <n v="181"/>
+    <n v="28"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="17.286000000000001"/>
+    <n v="399"/>
+    <n v="23"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="0.14299999999999999"/>
+    <n v="289"/>
+    <n v="57"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="3.286"/>
+    <n v="182"/>
+    <n v="47"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="1.571"/>
+    <n v="159"/>
+    <n v="31"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="19.713999999999999"/>
+    <n v="122"/>
+    <n v="27"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="126.714"/>
+    <n v="115"/>
+    <n v="61"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="8"/>
+    <n v="343"/>
+    <n v="60"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="71.713999999999999"/>
+    <n v="114"/>
+    <n v="28"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="63.713999999999999"/>
+    <n v="249"/>
+    <n v="36"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="96.286000000000001"/>
+    <n v="140"/>
+    <n v="29"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="50.856999999999999"/>
+    <n v="110"/>
+    <n v="34"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="155"/>
+    <n v="214"/>
+    <n v="49"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="39.570999999999998"/>
+    <n v="224"/>
+    <n v="45"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="36.286000000000001"/>
+    <n v="294"/>
+    <n v="28"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="102.571"/>
+    <n v="162"/>
+    <n v="24"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="8.1430000000000007"/>
+    <n v="140"/>
+    <n v="33"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="28"/>
+    <n v="147"/>
+    <n v="34"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="38"/>
+    <n v="138"/>
+    <n v="60"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="111.571"/>
+    <n v="196"/>
+    <n v="23"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="165"/>
+    <n v="139"/>
+    <n v="35"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="16"/>
+    <n v="246"/>
+    <n v="45"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="124.571"/>
+    <n v="105"/>
+    <n v="46"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="68"/>
+    <n v="160"/>
+    <n v="38"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="39.570999999999998"/>
+    <n v="146"/>
+    <n v="32"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="131"/>
+    <n v="187"/>
+    <n v="33"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="3.4289999999999998"/>
+    <n v="372"/>
+    <n v="52"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="42"/>
+    <n v="146"/>
+    <n v="50"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="26"/>
+    <n v="131"/>
+    <n v="38"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="37.856999999999999"/>
+    <n v="237"/>
+    <n v="47"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="92.713999999999999"/>
+    <n v="105"/>
+    <n v="23"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="106.714"/>
+    <n v="140"/>
+    <n v="31"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="11.143000000000001"/>
+    <n v="136"/>
+    <n v="55"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="115"/>
+    <n v="147"/>
+    <n v="39"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="44"/>
+    <n v="160"/>
+    <n v="41"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="75"/>
+    <n v="175"/>
+    <n v="62"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="77.856999999999999"/>
+    <n v="261"/>
+    <n v="50"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="0.28599999999999998"/>
+    <n v="146"/>
+    <n v="46"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="86"/>
+    <n v="195"/>
+    <n v="33"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="12.429"/>
+    <n v="476"/>
+    <n v="22"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="22"/>
+    <n v="441"/>
+    <n v="37"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="5.4290000000000003"/>
+    <n v="86"/>
+    <n v="40"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="No Recurrence"/>
+    <n v="67"/>
+    <n v="201"/>
+    <n v="22"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="3.4289999999999998"/>
+    <n v="130"/>
+    <n v="30"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="6.2859999999999996"/>
+    <n v="86"/>
+    <n v="63"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="5"/>
+    <n v="209"/>
+    <n v="40"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="5.2859999999999996"/>
+    <n v="214"/>
+    <n v="23"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="1"/>
+    <n v="72"/>
+    <n v="52"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="3.4289999999999998"/>
+    <n v="238"/>
+    <n v="23"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="6.5709999999999997"/>
+    <n v="133"/>
+    <n v="22"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="1"/>
+    <n v="128"/>
+    <n v="23"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="No Recurrence"/>
+    <n v="45"/>
+    <n v="139"/>
+    <n v="30"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="109.571"/>
+    <n v="148"/>
+    <n v="26"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="0.85699999999999998"/>
+    <n v="285"/>
+    <n v="46"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="4.7140000000000004"/>
+    <n v="141"/>
+    <n v="61"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="0.57099999999999995"/>
+    <n v="212"/>
+    <n v="30"/>
+    <s v="Male"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="9.1430000000000007"/>
+    <n v="168"/>
+    <n v="39"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="No Recurrence"/>
+    <n v="102"/>
+    <n v="305"/>
+    <n v="49"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="46.286000000000001"/>
+    <n v="204"/>
+    <n v="57"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="0.57099999999999995"/>
+    <n v="140"/>
+    <n v="51"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="6.4290000000000003"/>
+    <n v="182"/>
+    <n v="53"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="0"/>
+    <n v="162"/>
+    <n v="31"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="20.856999999999999"/>
+    <n v="207"/>
+    <n v="43"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Placebo"/>
+    <s v="Recurrence"/>
+    <n v="18.286000000000001"/>
+    <n v="102"/>
+    <n v="29"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="31.856999999999999"/>
+    <n v="154"/>
+    <n v="28"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Zoloft"/>
+    <s v="Recurrence"/>
+    <n v="22"/>
+    <n v="203"/>
+    <n v="51"/>
+    <s v="Female"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Prozac"/>
+    <s v="Recurrence"/>
+    <n v="2"/>
+    <n v="176"/>
+    <n v="33"/>
+    <s v="Female"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5E8AB82F-A5E6-4ACF-A5A1-4567672D83A2}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
+  <location ref="I3:J9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Hospt" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,106 +4225,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C534A9-ACB0-6645-9A2D-699004367EA5}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="142" workbookViewId="0"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="5"/>
+    <col min="3" max="16384" width="10.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="6">
         <v>5</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="6">
         <v>8</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="6">
         <v>9</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="6">
         <v>10</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -745,23 +4335,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="8.77734375" style="1"/>
+    <col min="9" max="9" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -783,19 +4376,19 @@
       <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="21"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="24"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -818,7 +4411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -840,8 +4433,15 @@
       <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -863,8 +4463,15 @@
       <c r="G4" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I4" s="11">
+        <v>1</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.16513761467889909</v>
+      </c>
+      <c r="K4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -886,8 +4493,15 @@
       <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I5" s="11">
+        <v>2</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.15596330275229359</v>
+      </c>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -909,8 +4523,15 @@
       <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I6" s="11">
+        <v>3</v>
+      </c>
+      <c r="J6" s="12">
+        <v>9.1743119266055051E-2</v>
+      </c>
+      <c r="K6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -932,8 +4553,15 @@
       <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I7" s="11">
+        <v>4</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0.34862385321100919</v>
+      </c>
+      <c r="K7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -955,8 +4583,15 @@
       <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I8" s="11">
+        <v>5</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0.23853211009174313</v>
+      </c>
+      <c r="K8"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -978,8 +4613,15 @@
       <c r="G9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="12">
+        <v>1</v>
+      </c>
+      <c r="K9"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1001,8 +4643,11 @@
       <c r="G10" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -1024,8 +4669,11 @@
       <c r="G11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -1047,8 +4695,11 @@
       <c r="G12" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -1070,8 +4721,11 @@
       <c r="G13" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>1</v>
       </c>
@@ -1093,8 +4747,11 @@
       <c r="G14" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>1</v>
       </c>
@@ -1116,8 +4773,11 @@
       <c r="G15" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1</v>
       </c>
@@ -1139,8 +4799,11 @@
       <c r="G16" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -1162,8 +4825,11 @@
       <c r="G17" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>1</v>
       </c>
@@ -1185,8 +4851,11 @@
       <c r="G18" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>1</v>
       </c>
@@ -1208,8 +4877,11 @@
       <c r="G19" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>2</v>
       </c>
@@ -1231,8 +4903,11 @@
       <c r="G20" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>2</v>
       </c>
@@ -1264,7 +4939,7 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>2</v>
       </c>
@@ -1287,7 +4962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>2</v>
       </c>
@@ -1310,7 +4985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2</v>
       </c>
@@ -1333,7 +5008,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>2</v>
       </c>
@@ -1356,7 +5031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>2</v>
       </c>
@@ -1379,7 +5054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>2</v>
       </c>
@@ -1402,7 +5077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>2</v>
       </c>
@@ -1425,7 +5100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>2</v>
       </c>
@@ -1448,7 +5123,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>2</v>
       </c>
@@ -1471,7 +5146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>2</v>
       </c>
@@ -1494,7 +5169,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>2</v>
       </c>
@@ -1517,7 +5192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>2</v>
       </c>
@@ -1540,7 +5215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>2</v>
       </c>
@@ -1563,7 +5238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>2</v>
       </c>
@@ -1586,7 +5261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>2</v>
       </c>
@@ -1609,7 +5284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>3</v>
       </c>
@@ -1632,7 +5307,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>3</v>
       </c>
@@ -1655,7 +5330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>3</v>
       </c>
@@ -1678,7 +5353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>3</v>
       </c>
@@ -1701,7 +5376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>3</v>
       </c>
@@ -1724,7 +5399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>3</v>
       </c>
@@ -1747,7 +5422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>3</v>
       </c>
@@ -1770,7 +5445,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>3</v>
       </c>
@@ -1793,7 +5468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>3</v>
       </c>
@@ -1816,7 +5491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>3</v>
       </c>
@@ -1839,7 +5514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>4</v>
       </c>
@@ -1862,7 +5537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>4</v>
       </c>
@@ -1885,7 +5560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>4</v>
       </c>
@@ -1908,7 +5583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>4</v>
       </c>
@@ -1931,7 +5606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>4</v>
       </c>
@@ -1954,7 +5629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>4</v>
       </c>
@@ -1977,7 +5652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>4</v>
       </c>
@@ -2000,7 +5675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>4</v>
       </c>
@@ -2023,7 +5698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>4</v>
       </c>
@@ -2046,7 +5721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>4</v>
       </c>
@@ -2069,7 +5744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>4</v>
       </c>
@@ -2092,7 +5767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>4</v>
       </c>
@@ -2115,7 +5790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>4</v>
       </c>
@@ -2138,7 +5813,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>4</v>
       </c>
@@ -2161,7 +5836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>4</v>
       </c>
@@ -2184,7 +5859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>4</v>
       </c>
@@ -2207,7 +5882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>4</v>
       </c>
@@ -2230,7 +5905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>4</v>
       </c>
@@ -2253,7 +5928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>4</v>
       </c>
@@ -2276,7 +5951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>4</v>
       </c>
@@ -2299,7 +5974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>4</v>
       </c>
@@ -2322,7 +5997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>4</v>
       </c>
@@ -2345,7 +6020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>4</v>
       </c>
@@ -2368,7 +6043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>4</v>
       </c>
@@ -2391,7 +6066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>4</v>
       </c>
@@ -2414,7 +6089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>4</v>
       </c>
@@ -2437,7 +6112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>4</v>
       </c>
@@ -2460,7 +6135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>4</v>
       </c>
@@ -2483,7 +6158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>4</v>
       </c>
@@ -2506,7 +6181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>4</v>
       </c>
@@ -2529,7 +6204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>4</v>
       </c>
@@ -2552,7 +6227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>4</v>
       </c>
@@ -2575,7 +6250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>4</v>
       </c>
@@ -2598,7 +6273,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>4</v>
       </c>
@@ -2621,7 +6296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>4</v>
       </c>
@@ -2644,7 +6319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>4</v>
       </c>
@@ -2667,7 +6342,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>4</v>
       </c>
@@ -2690,7 +6365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>4</v>
       </c>
@@ -2713,7 +6388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>5</v>
       </c>
@@ -2736,7 +6411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>5</v>
       </c>
@@ -2759,7 +6434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>5</v>
       </c>
@@ -2782,7 +6457,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>5</v>
       </c>
@@ -2805,7 +6480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>5</v>
       </c>
@@ -2828,7 +6503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>5</v>
       </c>
@@ -2851,7 +6526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>5</v>
       </c>
@@ -2874,7 +6549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>5</v>
       </c>
@@ -2897,7 +6572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>5</v>
       </c>
@@ -2920,7 +6595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>5</v>
       </c>
@@ -2943,7 +6618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>5</v>
       </c>
@@ -2966,7 +6641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>5</v>
       </c>
@@ -2989,7 +6664,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>5</v>
       </c>
@@ -3012,7 +6687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>5</v>
       </c>
@@ -3035,7 +6710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>5</v>
       </c>
@@ -3058,7 +6733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>5</v>
       </c>
@@ -3081,7 +6756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>5</v>
       </c>
@@ -3104,7 +6779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>5</v>
       </c>
@@ -3127,7 +6802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>5</v>
       </c>
@@ -3150,7 +6825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>5</v>
       </c>
@@ -3173,7 +6848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>5</v>
       </c>
@@ -3196,7 +6871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>5</v>
       </c>
@@ -3219,7 +6894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>5</v>
       </c>
@@ -3242,7 +6917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>5</v>
       </c>
@@ -3265,7 +6940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>5</v>
       </c>
@@ -3288,7 +6963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>5</v>
       </c>
@@ -3318,5 +6993,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>